<commit_message>
Botones de retroceso en usuario agregado
</commit_message>
<xml_diff>
--- a/Files/ElSaborAlejandro.xlsx
+++ b/Files/ElSaborAlejandro.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -637,6 +637,15 @@
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregadas ventanas de carrito y retroceso/vaciado
Vaciado de lista y agregado carrito
</commit_message>
<xml_diff>
--- a/Files/ElSaborAlejandro.xlsx
+++ b/Files/ElSaborAlejandro.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +646,186 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
     </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>